<commit_message>
Implemeted feature changes based on feedback
</commit_message>
<xml_diff>
--- a/extraFiles/DTT-Assessment-Hour-Log.xlsx
+++ b/extraFiles/DTT-Assessment-Hour-Log.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
   <si>
     <r>
       <rPr>
@@ -129,6 +129,82 @@
   </si>
   <si>
     <t>This was done simultaneously while working, but the overall time spent on this was around an hour</t>
+  </si>
+  <si>
+    <t>Spent time working on the following</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="12"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">- Indicated that output is of type JSON in the header, 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="12"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">Created collection variables for base url in postman, 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="12"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">Introduced path variables in postman urls </t>
+    </r>
+  </si>
+  <si>
+    <t>Improving documentation</t>
+  </si>
+  <si>
+    <t>Added PHPDoc style comments,</t>
+  </si>
+  <si>
+    <t>Made changes to the following features</t>
+  </si>
+  <si>
+    <t>Improved model logic, Facility names are no longer unique, Added input validation to prevent unwanted errors from occurring</t>
+  </si>
+  <si>
+    <t>Worked on the following features</t>
+  </si>
+  <si>
+    <t>- Changed createFacility logic to be more single responsibility, 
+- Facility names are no longer unique so multiple facilities with same name are now returned by getFacility, 
+- Searching for facilities now returns all associated tags</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="8"/>
+        <rFont val="Open Sans"/>
+      </rPr>
+      <t xml:space="preserve">- updateFacility and deleteFacility now check on id instead of name,
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="8"/>
+        <rFont val="Open Sans"/>
+      </rPr>
+      <t>Changed getAllFacilities logic to re-use searchFacilitiesByFilter logic with no filters applied</t>
+    </r>
+  </si>
+  <si>
+    <t>Updating spreadsheet</t>
+  </si>
+  <si>
+    <t>This was also done simultaneously while working. Estimated time is 30 minutes. The spreadsheet rounds off 0.5 to 1 in hours column</t>
   </si>
   <si>
     <t>Total amount of hours</t>
@@ -142,7 +218,7 @@
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="59" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -179,6 +255,16 @@
       <name val="Open Sans"/>
     </font>
     <font>
+      <sz val="8"/>
+      <color indexed="12"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="8"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Open Sans"/>
@@ -204,7 +290,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -287,7 +373,7 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="10"/>
       </right>
       <top/>
       <bottom/>
@@ -295,21 +381,36 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="10"/>
       </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="8"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
       <right style="thin">
         <color indexed="8"/>
       </right>
@@ -325,6 +426,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="8"/>
       </left>
@@ -338,7 +448,9 @@
         <color indexed="8"/>
       </left>
       <right/>
-      <top/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
       <bottom style="thin">
         <color indexed="8"/>
       </bottom>
@@ -359,6 +471,26 @@
         <color indexed="8"/>
       </right>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="8"/>
       </bottom>
@@ -370,7 +502,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -389,6 +521,9 @@
     <xf numFmtId="1" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -398,52 +533,100 @@
     <xf numFmtId="1" fontId="3" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="59" fontId="5" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="justify" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="5" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="5" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="9" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="1" fontId="3" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -466,6 +649,7 @@
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffeb5340"/>
+      <rgbColor rgb="ff222222"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -653,13 +837,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -758,10 +936,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1016,13 +1194,7 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
+        <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -1335,10 +1507,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1589,7 +1761,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1599,8 +1771,8 @@
     <col min="2" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="3" width="8.625" style="1" customWidth="1"/>
     <col min="4" max="4" width="38.625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="6.5" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="6.5" style="1" customWidth="1"/>
+    <col min="5" max="8" width="6.5" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="6.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="73.5" customHeight="1">
@@ -1610,399 +1782,515 @@
       <c r="D1" s="3"/>
       <c r="E1" s="4"/>
       <c r="F1" s="5"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
     </row>
     <row r="2" ht="46.5" customHeight="1">
-      <c r="A2" t="s" s="6">
+      <c r="A2" t="s" s="7">
         <v>0</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="7"/>
     </row>
     <row r="3" ht="16.5" customHeight="1">
-      <c r="A3" t="s" s="9">
+      <c r="A3" t="s" s="11">
         <v>1</v>
       </c>
-      <c r="B3" t="s" s="9">
+      <c r="B3" t="s" s="11">
         <v>2</v>
       </c>
-      <c r="C3" t="s" s="9">
+      <c r="C3" t="s" s="11">
         <v>3</v>
       </c>
-      <c r="D3" t="s" s="9">
+      <c r="D3" t="s" s="11">
         <v>4</v>
       </c>
-      <c r="E3" t="s" s="9">
+      <c r="E3" t="s" s="11">
         <v>5</v>
       </c>
-      <c r="F3" s="10"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
     </row>
     <row r="4" ht="37" customHeight="1">
-      <c r="A4" t="s" s="11">
+      <c r="A4" t="s" s="13">
         <v>6</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="14">
         <v>1</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="15">
         <v>45300</v>
       </c>
-      <c r="D4" t="s" s="11">
+      <c r="D4" t="s" s="16">
         <v>7</v>
       </c>
-      <c r="E4" s="14"/>
-      <c r="F4" s="10"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
     </row>
     <row r="5" ht="23" customHeight="1">
-      <c r="A5" t="s" s="11">
+      <c r="A5" t="s" s="13">
         <v>8</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="14">
         <v>1</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="15">
         <v>45300</v>
       </c>
-      <c r="D5" t="s" s="11">
+      <c r="D5" t="s" s="16">
         <v>9</v>
       </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="10"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
     </row>
     <row r="6" ht="30.05" customHeight="1">
-      <c r="A6" t="s" s="11">
+      <c r="A6" t="s" s="13">
         <v>10</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="14">
         <v>1</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="15">
         <v>45301</v>
       </c>
-      <c r="D6" t="s" s="11">
+      <c r="D6" t="s" s="16">
         <v>11</v>
       </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="10"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
     </row>
     <row r="7" ht="33" customHeight="1">
-      <c r="A7" t="s" s="11">
+      <c r="A7" t="s" s="13">
         <v>12</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="14">
         <v>3</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="15">
         <v>45301</v>
       </c>
-      <c r="D7" t="s" s="11">
+      <c r="D7" t="s" s="16">
         <v>13</v>
       </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="10"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
     </row>
     <row r="8" ht="23" customHeight="1">
-      <c r="A8" t="s" s="11">
+      <c r="A8" t="s" s="13">
         <v>14</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="14">
         <v>2</v>
       </c>
-      <c r="C8" s="13">
-        <v>45302</v>
-      </c>
-      <c r="D8" t="s" s="11">
+      <c r="C8" s="15">
+        <v>45668</v>
+      </c>
+      <c r="D8" t="s" s="16">
         <v>15</v>
       </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="10"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
     </row>
     <row r="9" ht="23" customHeight="1">
-      <c r="A9" t="s" s="11">
+      <c r="A9" t="s" s="13">
         <v>16</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="14">
         <v>2</v>
       </c>
-      <c r="C9" s="13">
-        <v>45302</v>
-      </c>
-      <c r="D9" t="s" s="11">
+      <c r="C9" s="15">
+        <v>45668</v>
+      </c>
+      <c r="D9" t="s" s="16">
         <v>17</v>
       </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="10"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
     </row>
     <row r="10" ht="23" customHeight="1">
-      <c r="A10" t="s" s="11">
+      <c r="A10" t="s" s="13">
         <v>18</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="14">
         <v>1</v>
       </c>
-      <c r="C10" s="13">
-        <v>45302</v>
-      </c>
-      <c r="D10" t="s" s="11">
+      <c r="C10" s="15">
+        <v>45668</v>
+      </c>
+      <c r="D10" t="s" s="16">
         <v>19</v>
       </c>
-      <c r="E10" t="s" s="14">
+      <c r="E10" t="s" s="17">
         <v>20</v>
       </c>
-      <c r="F10" s="10"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
     </row>
     <row r="11" ht="23" customHeight="1">
-      <c r="A11" t="s" s="11">
+      <c r="A11" t="s" s="13">
         <v>21</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="14">
         <v>2</v>
       </c>
-      <c r="C11" s="13">
-        <v>45303</v>
-      </c>
-      <c r="D11" t="s" s="11">
+      <c r="C11" s="15">
+        <v>45669</v>
+      </c>
+      <c r="D11" t="s" s="16">
         <v>22</v>
       </c>
-      <c r="E11" t="s" s="14">
+      <c r="E11" t="s" s="17">
         <v>20</v>
       </c>
-      <c r="F11" s="10"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
     </row>
     <row r="12" ht="17" customHeight="1">
-      <c r="A12" t="s" s="11">
+      <c r="A12" t="s" s="13">
         <v>23</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="14">
         <v>1</v>
       </c>
-      <c r="C12" s="13">
-        <v>45304</v>
-      </c>
-      <c r="D12" t="s" s="11">
+      <c r="C12" s="15">
+        <v>45670</v>
+      </c>
+      <c r="D12" t="s" s="16">
         <v>24</v>
       </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="10"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
     </row>
     <row r="13" ht="23" customHeight="1">
-      <c r="A13" t="s" s="11">
+      <c r="A13" t="s" s="13">
         <v>25</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="14">
         <v>2</v>
       </c>
-      <c r="C13" s="13">
-        <v>45304</v>
-      </c>
-      <c r="D13" t="s" s="11">
+      <c r="C13" s="15">
+        <v>45670</v>
+      </c>
+      <c r="D13" t="s" s="16">
         <v>26</v>
       </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="10"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
     </row>
     <row r="14" ht="23" customHeight="1">
-      <c r="A14" t="s" s="11">
+      <c r="A14" t="s" s="13">
         <v>27</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="14">
         <v>1</v>
       </c>
-      <c r="C14" s="13">
-        <v>45305</v>
-      </c>
-      <c r="D14" t="s" s="11">
+      <c r="C14" s="15">
+        <v>45671</v>
+      </c>
+      <c r="D14" t="s" s="16">
         <v>28</v>
       </c>
-      <c r="E14" s="14"/>
-      <c r="F14" s="10"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
     </row>
     <row r="15" ht="23" customHeight="1">
-      <c r="A15" t="s" s="11">
+      <c r="A15" t="s" s="13">
         <v>29</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15" s="14">
         <v>1</v>
       </c>
-      <c r="C15" s="13">
-        <v>45305</v>
-      </c>
-      <c r="D15" t="s" s="11">
+      <c r="C15" s="15">
+        <v>45671</v>
+      </c>
+      <c r="D15" t="s" s="16">
         <v>30</v>
       </c>
-      <c r="E15" s="14"/>
-      <c r="F15" s="10"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
     </row>
     <row r="16" ht="23" customHeight="1">
-      <c r="A16" t="s" s="11">
+      <c r="A16" t="s" s="13">
         <v>31</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B16" s="14">
         <v>1</v>
       </c>
-      <c r="C16" s="13">
-        <v>45305</v>
-      </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="10"/>
+      <c r="C16" s="15">
+        <v>45671</v>
+      </c>
+      <c r="D16" s="16"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
     </row>
     <row r="17" ht="23" customHeight="1">
-      <c r="A17" t="s" s="11">
+      <c r="A17" t="s" s="13">
         <v>32</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17" s="14">
         <v>1</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" t="s" s="11">
+      <c r="C17" s="15">
+        <v>45686</v>
+      </c>
+      <c r="D17" t="s" s="16">
         <v>33</v>
       </c>
-      <c r="E17" s="14"/>
-      <c r="F17" s="10"/>
-    </row>
-    <row r="18" ht="16.5" customHeight="1">
-      <c r="A18" s="11"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="10"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+    </row>
+    <row r="18" ht="39.25" customHeight="1">
+      <c r="A18" t="s" s="13">
+        <v>34</v>
+      </c>
+      <c r="B18" s="14">
+        <v>1</v>
+      </c>
+      <c r="C18" s="15">
+        <v>45687</v>
+      </c>
+      <c r="D18" t="s" s="18">
+        <v>35</v>
+      </c>
+      <c r="E18" s="19"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="21"/>
     </row>
     <row r="19" ht="16.5" customHeight="1">
-      <c r="A19" s="11"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="10"/>
-    </row>
-    <row r="20" ht="16.5" customHeight="1">
-      <c r="A20" s="11"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="10"/>
-    </row>
-    <row r="21" ht="16.5" customHeight="1">
-      <c r="A21" s="11"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="10"/>
-    </row>
-    <row r="22" ht="16.5" customHeight="1">
-      <c r="A22" s="11"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="10"/>
-    </row>
-    <row r="23" ht="16.5" customHeight="1">
-      <c r="A23" s="11"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="10"/>
+      <c r="A19" t="s" s="13">
+        <v>36</v>
+      </c>
+      <c r="B19" s="14">
+        <v>1</v>
+      </c>
+      <c r="C19" s="15">
+        <v>45690</v>
+      </c>
+      <c r="D19" t="s" s="16">
+        <v>37</v>
+      </c>
+      <c r="E19" s="22"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="21"/>
+    </row>
+    <row r="20" ht="23" customHeight="1">
+      <c r="A20" t="s" s="13">
+        <v>38</v>
+      </c>
+      <c r="B20" s="14">
+        <v>1</v>
+      </c>
+      <c r="C20" s="15">
+        <v>45691</v>
+      </c>
+      <c r="D20" t="s" s="16">
+        <v>39</v>
+      </c>
+      <c r="E20" s="22"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="21"/>
+    </row>
+    <row r="21" ht="43" customHeight="1">
+      <c r="A21" t="s" s="13">
+        <v>40</v>
+      </c>
+      <c r="B21" s="14">
+        <v>1</v>
+      </c>
+      <c r="C21" s="15">
+        <v>45692</v>
+      </c>
+      <c r="D21" t="s" s="16">
+        <v>41</v>
+      </c>
+      <c r="E21" s="22"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="21"/>
+    </row>
+    <row r="22" ht="33" customHeight="1">
+      <c r="A22" t="s" s="13">
+        <v>40</v>
+      </c>
+      <c r="B22" s="14">
+        <v>1</v>
+      </c>
+      <c r="C22" s="15">
+        <v>45692</v>
+      </c>
+      <c r="D22" t="s" s="16">
+        <v>42</v>
+      </c>
+      <c r="E22" s="22"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="21"/>
+    </row>
+    <row r="23" ht="23" customHeight="1">
+      <c r="A23" t="s" s="13">
+        <v>43</v>
+      </c>
+      <c r="B23" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="C23" s="15"/>
+      <c r="D23" t="s" s="23">
+        <v>44</v>
+      </c>
+      <c r="E23" s="24"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="26"/>
     </row>
     <row r="24" ht="16.5" customHeight="1">
-      <c r="A24" s="11"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="10"/>
+      <c r="A24" s="27"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
     </row>
     <row r="25" ht="16.5" customHeight="1">
-      <c r="A25" s="11"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="10"/>
+      <c r="A25" s="27"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
     </row>
     <row r="26" ht="16.5" customHeight="1">
-      <c r="A26" s="11"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="10"/>
+      <c r="A26" s="27"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
     </row>
     <row r="27" ht="16.5" customHeight="1">
-      <c r="A27" s="11"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="10"/>
+      <c r="A27" s="27"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
     </row>
     <row r="28" ht="16.5" customHeight="1">
-      <c r="A28" s="11"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="10"/>
+      <c r="A28" s="27"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
     </row>
     <row r="29" ht="16.5" customHeight="1">
-      <c r="A29" s="11"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="10"/>
+      <c r="A29" s="28"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="15"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="17"/>
+      <c r="A30" s="31"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" t="s" s="18">
-        <v>34</v>
-      </c>
-      <c r="B31" s="19">
+      <c r="A31" t="s" s="34">
+        <v>45</v>
+      </c>
+      <c r="B31" s="35">
         <f>SUMIF(E4:E29,"&lt;&gt;x",B4:B29)</f>
-        <v>17</v>
-      </c>
-      <c r="C31" s="16"/>
+        <v>22.5</v>
+      </c>
+      <c r="C31" s="32"/>
       <c r="D31" s="4"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="17"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="16"/>
+      <c r="A32" s="32"/>
       <c r="B32" s="4"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="17"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="21"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="17"/>
+      <c r="A33" s="37"/>
+      <c r="B33" s="36"/>
+      <c r="C33" s="36"/>
+      <c r="D33" s="36"/>
+      <c r="E33" s="36"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="22"/>
-      <c r="B34" s="23"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="24"/>
+      <c r="A34" s="38"/>
+      <c r="B34" s="39"/>
+      <c r="C34" s="39"/>
+      <c r="D34" s="39"/>
+      <c r="E34" s="39"/>
+      <c r="F34" s="40"/>
+      <c r="G34" s="41"/>
+      <c r="H34" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>